<commit_message>
update raw data & rerun
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates_mp1_datasheet_Doue la Fontaine.xlsx
+++ b/data/raw_data/ManyPrimates_mp1_datasheet_Doue la Fontaine.xlsx
@@ -30333,7 +30333,7 @@
         <v>3.0</v>
       </c>
       <c r="O14" s="16">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="P14" s="16">
         <v>0.0</v>
@@ -30389,7 +30389,7 @@
         <v>2.0</v>
       </c>
       <c r="P15" s="16">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q15" s="15" t="s">
         <v>42</v>
@@ -30439,10 +30439,10 @@
         <v>1.0</v>
       </c>
       <c r="O16" s="16">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="P16" s="16">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q16" s="15" t="s">
         <v>42</v>

</xml_diff>